<commit_message>
GetByAdmissionRollAsync() Method Created and name changed to GetHonsByAdmissionRollAsync()
</commit_message>
<xml_diff>
--- a/OnlineAdmission.APP/wwwroot/FIleData/Tejgaon-College_Masters_Subject_Id-1051_29-11-2021_19-31-09.xlsx
+++ b/OnlineAdmission.APP/wwwroot/FIleData/Tejgaon-College_Masters_Subject_Id-1051_29-11-2021_19-31-09.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habib\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="14865" windowHeight="8580"/>
   </bookViews>
@@ -229,9 +224,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -279,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,7 +306,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -525,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -534,7 +526,7 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>